<commit_message>
Modificacion de escenarios de prueba
</commit_message>
<xml_diff>
--- a/report/Reporte de mutantes encontrados.xlsx
+++ b/report/Reporte de mutantes encontrados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
     <t xml:space="preserve">Mutante</t>
   </si>
@@ -133,8 +133,8 @@
   </sheetPr>
   <dimension ref="A1:B901"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B103" activeCellId="0" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -666,10 +666,16 @@
       <c r="A101" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B101" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
         <v>101</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>